<commit_message>
Test Case added under Script for valid and invalid login.  Updated the excel sheet path under env variable.
</commit_message>
<xml_diff>
--- a/Data/input.xlsx
+++ b/Data/input.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Automation\Selenium\day41\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8503E746-6FBB-49CC-AC39-AC85668C6313}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C841EE58-167E-4F39-B540-F768E263E99F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{CBF46EE8-0D20-4DF1-A789-1CBE8A19ED1E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ValidLogin" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,6 +30,20 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>UserNamePassword</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>manager</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -379,12 +393,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CEE3FF1-1FB8-4A7D-843C-00446AA4033F}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Invalid code to Login POM Class Added new sheet to excel Created new InvalidLogin test class updated IAUtoConst for excel sheet
</commit_message>
<xml_diff>
--- a/Data/input.xlsx
+++ b/Data/input.xlsx
@@ -1,47 +1,49 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Automation\Selenium\day41\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\B45\workspace\framework\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C841EE58-167E-4F39-B540-F768E263E99F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C9EC770-2FCD-488F-88AE-6438BE144525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{CBF46EE8-0D20-4DF1-A789-1CBE8A19ED1E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ValidLogin" sheetId="1" r:id="rId1"/>
+    <sheet name="InvalidLogin" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>UserNamePassword</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Password</t>
   </si>
   <si>
     <t>admin</t>
   </si>
   <si>
     <t>manager</t>
+  </si>
+  <si>
+    <t>Bhanu</t>
+  </si>
+  <si>
+    <t>Damager</t>
   </si>
 </sst>
 </file>
@@ -113,7 +115,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -125,7 +127,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -172,23 +174,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -224,23 +209,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -392,26 +360,64 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CEE3FF1-1FB8-4A7D-843C-00446AA4033F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CB012FF-C06C-46EA-8E62-160A274A898D}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>